<commit_message>
Foot Keypoint no Value
</commit_message>
<xml_diff>
--- a/results/idealsitups-summary.xlsx
+++ b/results/idealsitups-summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>M-bert-situps.mp4</t>
+          <t>M-situps.mp4</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -491,64 +491,6 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>M-don-situps.mp4</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Poor</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Limited</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>M-situps.mp4</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Poor</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Limited</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>